<commit_message>
Adicionando cadastros novos e modelagem do script
</commit_message>
<xml_diff>
--- a/Documentação/BacklogDeRequisitos.xlsx
+++ b/Documentação/BacklogDeRequisitos.xlsx
@@ -342,35 +342,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -718,7 +718,7 @@
   <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -734,46 +734,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="9"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="13"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
     </row>
     <row r="2" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -793,7 +793,7 @@
       <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="7" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="2">
@@ -819,7 +819,7 @@
       <c r="F4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="9" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="2">
@@ -845,7 +845,7 @@
       <c r="F5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="9" t="s">
         <v>14</v>
       </c>
       <c r="H5" s="2">
@@ -871,7 +871,7 @@
       <c r="F6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="8" t="s">
         <v>18</v>
       </c>
       <c r="H6" s="2">
@@ -897,7 +897,7 @@
       <c r="F7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="9" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="2">
@@ -924,7 +924,7 @@
       <c r="F8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="9" t="s">
         <v>14</v>
       </c>
       <c r="H8" s="2">
@@ -934,7 +934,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
         <v>8</v>
@@ -951,7 +951,7 @@
       <c r="F9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="8" t="s">
         <v>18</v>
       </c>
       <c r="H9" s="2">
@@ -977,7 +977,7 @@
       <c r="F10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="8" t="s">
         <v>18</v>
       </c>
       <c r="H10" s="2">
@@ -1004,7 +1004,7 @@
       <c r="F11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="7" t="s">
         <v>12</v>
       </c>
       <c r="H11" s="2">

</xml_diff>